<commit_message>
Finished the analytics part
</commit_message>
<xml_diff>
--- a/outputs/sectorbreakdown.xlsx
+++ b/outputs/sectorbreakdown.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -430,37 +430,37 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.879</v>
+        <v>-13.74</v>
       </c>
       <c r="C2" t="n">
-        <v>3.574</v>
+        <v>-5.307</v>
       </c>
       <c r="D2" t="n">
-        <v>-5.395</v>
+        <v>-19.793</v>
       </c>
       <c r="E2" t="n">
-        <v>-30.077</v>
+        <v>-2.772</v>
       </c>
       <c r="F2" t="n">
-        <v>9.121</v>
+        <v>-10.347</v>
       </c>
       <c r="G2" t="n">
-        <v>1.042</v>
+        <v>-7.474</v>
       </c>
       <c r="H2" t="n">
-        <v>2.805</v>
+        <v>-10.866</v>
       </c>
       <c r="I2" t="n">
-        <v>-6.717</v>
+        <v>-7.366</v>
       </c>
       <c r="J2" t="n">
-        <v>1.07</v>
+        <v>-1.97</v>
       </c>
       <c r="K2" t="n">
-        <v>9.369999999999999</v>
+        <v>-11.217</v>
       </c>
       <c r="L2" t="n">
-        <v>9.747999999999999</v>
+        <v>-6.293</v>
       </c>
     </row>
     <row r="3">
@@ -470,37 +470,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.026</v>
+        <v>-15.363</v>
       </c>
       <c r="C3" t="n">
-        <v>6.015</v>
+        <v>-5.636</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.326</v>
+        <v>-21.774</v>
       </c>
       <c r="E3" t="n">
-        <v>-27.539</v>
+        <v>5.745</v>
       </c>
       <c r="F3" t="n">
-        <v>12.436</v>
+        <v>-9.612</v>
       </c>
       <c r="G3" t="n">
-        <v>-5.399</v>
+        <v>-4.655</v>
       </c>
       <c r="H3" t="n">
-        <v>7.55</v>
+        <v>-6.598</v>
       </c>
       <c r="I3" t="n">
-        <v>-2.235</v>
+        <v>2.533</v>
       </c>
       <c r="J3" t="n">
-        <v>8.843999999999999</v>
+        <v>0.091</v>
       </c>
       <c r="K3" t="n">
-        <v>14.062</v>
+        <v>-3.924</v>
       </c>
       <c r="L3" t="n">
-        <v>9.747999999999999</v>
+        <v>-2.214</v>
       </c>
     </row>
     <row r="4">
@@ -510,37 +510,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>16.206</v>
+        <v>-13.807</v>
       </c>
       <c r="C4" t="n">
-        <v>31.78</v>
+        <v>-5.562</v>
       </c>
       <c r="D4" t="n">
-        <v>-2.572</v>
+        <v>-24.224</v>
       </c>
       <c r="E4" t="n">
-        <v>-3.87</v>
+        <v>0.825</v>
       </c>
       <c r="F4" t="n">
-        <v>44.183</v>
+        <v>-9.202</v>
       </c>
       <c r="G4" t="n">
-        <v>1.187</v>
+        <v>-5.167</v>
       </c>
       <c r="H4" t="n">
-        <v>40.116</v>
+        <v>-7.841</v>
       </c>
       <c r="I4" t="n">
-        <v>13.577</v>
+        <v>-0.593</v>
       </c>
       <c r="J4" t="n">
-        <v>15.397</v>
+        <v>-2.782</v>
       </c>
       <c r="K4" t="n">
-        <v>11.722</v>
+        <v>-7.328</v>
       </c>
       <c r="L4" t="n">
-        <v>-2.258</v>
+        <v>-2.96</v>
       </c>
     </row>
     <row r="5">
@@ -550,37 +550,37 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7.46</v>
+        <v>-13.424</v>
       </c>
       <c r="C5" t="n">
-        <v>28.865</v>
+        <v>10.607</v>
       </c>
       <c r="D5" t="n">
-        <v>-10.197</v>
+        <v>-29.568</v>
       </c>
       <c r="E5" t="n">
-        <v>-5.983</v>
+        <v>22.34</v>
       </c>
       <c r="F5" t="n">
-        <v>35.523</v>
+        <v>2.433</v>
       </c>
       <c r="G5" t="n">
-        <v>-9.260999999999999</v>
+        <v>5.527</v>
       </c>
       <c r="H5" t="n">
-        <v>26.444</v>
+        <v>14.033</v>
       </c>
       <c r="I5" t="n">
-        <v>8.236000000000001</v>
+        <v>-76.22499999999999</v>
       </c>
       <c r="J5" t="n">
-        <v>12.029</v>
+        <v>6.107</v>
       </c>
       <c r="K5" t="n">
-        <v>13.604</v>
+        <v>13.438</v>
       </c>
       <c r="L5" t="n">
-        <v>-3.535</v>
+        <v>-11.549</v>
       </c>
     </row>
     <row r="6">
@@ -590,34 +590,38 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>29.84</v>
+        <v>-17.161</v>
       </c>
       <c r="C6" t="n">
-        <v>57.002</v>
+        <v>34.593</v>
       </c>
       <c r="D6" t="n">
-        <v>-16.388</v>
+        <v>14.897</v>
       </c>
       <c r="E6" t="n">
-        <v>55.392</v>
+        <v>-7.182</v>
       </c>
       <c r="F6" t="n">
-        <v>89.843</v>
+        <v>40.312</v>
       </c>
       <c r="G6" t="n">
-        <v>30.35</v>
+        <v>-9.246</v>
       </c>
       <c r="H6" t="n">
-        <v>18.483</v>
+        <v>-17.719</v>
       </c>
       <c r="I6" t="n">
-        <v>19.924</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
+        <v>-499.751</v>
+      </c>
+      <c r="J6" t="n">
+        <v>15.991</v>
+      </c>
       <c r="K6" t="n">
-        <v>43.759</v>
-      </c>
-      <c r="L6" t="inlineStr"/>
+        <v>57.695</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-10.639</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -626,34 +630,36 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6.516</v>
+        <v>-4.178</v>
       </c>
       <c r="C7" t="n">
-        <v>11.52</v>
+        <v>6.967</v>
       </c>
       <c r="D7" t="n">
-        <v>-4.234</v>
+        <v>3.198</v>
       </c>
       <c r="E7" t="n">
-        <v>11.243</v>
+        <v>-1.675</v>
       </c>
       <c r="F7" t="n">
-        <v>16.76</v>
+        <v>7.981</v>
       </c>
       <c r="G7" t="n">
-        <v>6.617</v>
+        <v>-2.175</v>
       </c>
       <c r="H7" t="n">
-        <v>4.185</v>
-      </c>
-      <c r="I7" t="n">
-        <v>4.49</v>
-      </c>
-      <c r="J7" t="inlineStr"/>
+        <v>-4.325</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>3.42</v>
+      </c>
       <c r="K7" t="n">
-        <v>9.17</v>
-      </c>
-      <c r="L7" t="inlineStr"/>
+        <v>10.878</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-2.518</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -662,37 +668,37 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>73057.82000000001</v>
+        <v>64367.21</v>
       </c>
       <c r="C8" t="n">
-        <v>171460.08</v>
+        <v>166301.59</v>
       </c>
       <c r="D8" t="n">
-        <v>83349.36</v>
+        <v>66788.39</v>
       </c>
       <c r="E8" t="n">
-        <v>65589.95</v>
+        <v>46738.05</v>
       </c>
       <c r="F8" t="n">
-        <v>172543.04</v>
+        <v>198680.39</v>
       </c>
       <c r="G8" t="n">
-        <v>159377.64</v>
+        <v>135461.86</v>
       </c>
       <c r="H8" t="n">
-        <v>153183.81</v>
+        <v>144106.07</v>
       </c>
       <c r="I8" t="n">
-        <v>78237.25999999999</v>
+        <v>74203.16</v>
       </c>
       <c r="J8" t="n">
-        <v>58397.01</v>
+        <v>48487.82</v>
       </c>
       <c r="K8" t="n">
-        <v>206584.12</v>
+        <v>260273.99</v>
       </c>
       <c r="L8" t="n">
-        <v>60466.84</v>
+        <v>22371.09</v>
       </c>
     </row>
     <row r="9">
@@ -702,37 +708,37 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.729</v>
+        <v>0.722</v>
       </c>
       <c r="C9" t="n">
-        <v>1.013</v>
+        <v>0.996</v>
       </c>
       <c r="D9" t="n">
-        <v>1.159</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5570000000000001</v>
+        <v>0.619</v>
       </c>
       <c r="F9" t="n">
         <v>0.917</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9379999999999999</v>
+        <v>0.996</v>
       </c>
       <c r="H9" t="n">
-        <v>0.853</v>
+        <v>0.986</v>
       </c>
       <c r="I9" t="n">
-        <v>0.475</v>
+        <v>-0.028</v>
       </c>
       <c r="J9" t="n">
-        <v>0.863</v>
+        <v>0.663</v>
       </c>
       <c r="K9" t="n">
-        <v>1.136</v>
+        <v>1.101</v>
       </c>
       <c r="L9" t="n">
-        <v>0.667</v>
+        <v>0.468</v>
       </c>
     </row>
     <row r="10">
@@ -742,34 +748,36 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.199</v>
+        <v>-10.318</v>
       </c>
       <c r="C10" t="n">
-        <v>3.441</v>
+        <v>-1.008</v>
       </c>
       <c r="D10" t="n">
-        <v>-13.22</v>
+        <v>-4.394</v>
       </c>
       <c r="E10" t="n">
-        <v>5.996</v>
+        <v>-7.122</v>
       </c>
       <c r="F10" t="n">
-        <v>9.275</v>
+        <v>0.539</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.001</v>
+        <v>-10.152</v>
       </c>
       <c r="H10" t="n">
-        <v>-2.901</v>
-      </c>
-      <c r="I10" t="n">
-        <v>-0.252</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
+        <v>-12.231</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="n">
+        <v>-2.324</v>
+      </c>
       <c r="K10" t="n">
-        <v>0.327</v>
-      </c>
-      <c r="L10" t="inlineStr"/>
+        <v>2.203</v>
+      </c>
+      <c r="L10" t="n">
+        <v>-6.953</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -778,34 +786,36 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.063</v>
+        <v>-31.689</v>
       </c>
       <c r="C11" t="n">
-        <v>0.349</v>
+        <v>34.964</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.11</v>
+        <v>3.146</v>
       </c>
       <c r="E11" t="n">
-        <v>0.129</v>
+        <v>-11.166</v>
       </c>
       <c r="F11" t="n">
-        <v>0.447</v>
+        <v>45.694</v>
       </c>
       <c r="G11" t="n">
-        <v>0.06900000000000001</v>
+        <v>-16.241</v>
       </c>
       <c r="H11" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="J11" t="inlineStr"/>
+        <v>-25.072</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="n">
+        <v>17.888</v>
+      </c>
       <c r="K11" t="n">
-        <v>0.261</v>
-      </c>
-      <c r="L11" t="inlineStr"/>
+        <v>49.357</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-23.774</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -814,34 +824,36 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.065</v>
+        <v>-0.076</v>
       </c>
       <c r="C12" t="n">
-        <v>0.096</v>
+        <v>0.057</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.052</v>
+        <v>0.02</v>
       </c>
       <c r="E12" t="n">
-        <v>0.17</v>
+        <v>-0.048</v>
       </c>
       <c r="F12" t="n">
-        <v>0.163</v>
+        <v>0.073</v>
       </c>
       <c r="G12" t="n">
-        <v>0.051</v>
+        <v>-0.035</v>
       </c>
       <c r="H12" t="n">
-        <v>0.028</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.057</v>
-      </c>
-      <c r="J12" t="inlineStr"/>
+        <v>-0.057</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
+        <v>0.032</v>
+      </c>
       <c r="K12" t="n">
-        <v>0.065</v>
-      </c>
-      <c r="L12" t="inlineStr"/>
+        <v>0.08699999999999999</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-0.082</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -850,37 +862,37 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-64.979</v>
+        <v>-35.044</v>
       </c>
       <c r="C13" t="n">
-        <v>-28.862</v>
+        <v>-25.478</v>
       </c>
       <c r="D13" t="n">
-        <v>-52.025</v>
+        <v>-36.952</v>
       </c>
       <c r="E13" t="n">
-        <v>-55.497</v>
+        <v>-48.448</v>
       </c>
       <c r="F13" t="n">
-        <v>-24.889</v>
+        <v>-21.505</v>
       </c>
       <c r="G13" t="n">
-        <v>-49.197</v>
+        <v>-26.76</v>
       </c>
       <c r="H13" t="n">
-        <v>-41.752</v>
+        <v>-43.575</v>
       </c>
       <c r="I13" t="n">
-        <v>-75.009</v>
+        <v>-1369.897</v>
       </c>
       <c r="J13" t="n">
-        <v>-22.591</v>
+        <v>-23.868</v>
       </c>
       <c r="K13" t="n">
-        <v>-44.589</v>
+        <v>-33.072</v>
       </c>
       <c r="L13" t="n">
-        <v>-23.342</v>
+        <v>-22.812</v>
       </c>
     </row>
     <row r="14">
@@ -890,37 +902,37 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>53.476</v>
+        <v>17.296</v>
       </c>
       <c r="C14" t="n">
-        <v>27.256</v>
+        <v>16.216</v>
       </c>
       <c r="D14" t="n">
-        <v>54.782</v>
+        <v>60.363</v>
       </c>
       <c r="E14" t="n">
-        <v>72.72</v>
+        <v>26.659</v>
       </c>
       <c r="F14" t="n">
-        <v>29.31</v>
+        <v>14.628</v>
       </c>
       <c r="G14" t="n">
-        <v>36.7</v>
+        <v>21.41</v>
       </c>
       <c r="H14" t="n">
-        <v>41.211</v>
+        <v>22.445</v>
       </c>
       <c r="I14" t="n">
-        <v>83.554</v>
+        <v>631.391</v>
       </c>
       <c r="J14" t="n">
-        <v>27.697</v>
+        <v>11.861</v>
       </c>
       <c r="K14" t="n">
-        <v>27.346</v>
+        <v>19.415</v>
       </c>
       <c r="L14" t="n">
-        <v>17.229</v>
+        <v>16.082</v>
       </c>
     </row>
     <row r="15">
@@ -930,37 +942,37 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.021</v>
+        <v>0.201</v>
       </c>
       <c r="C15" t="n">
-        <v>0.24</v>
+        <v>0.622</v>
       </c>
       <c r="D15" t="n">
-        <v>0.08799999999999999</v>
+        <v>0.081</v>
       </c>
       <c r="E15" t="n">
-        <v>0.004</v>
+        <v>0.067</v>
       </c>
       <c r="F15" t="n">
-        <v>0.153</v>
+        <v>0.666</v>
       </c>
       <c r="G15" t="n">
-        <v>0.105</v>
+        <v>0.32</v>
       </c>
       <c r="H15" t="n">
-        <v>0.061</v>
+        <v>0.252</v>
       </c>
       <c r="I15" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>0.141</v>
+        <v>0.672</v>
       </c>
       <c r="K15" t="n">
-        <v>0.332</v>
+        <v>0.663</v>
       </c>
       <c r="L15" t="n">
-        <v>0.145</v>
+        <v>0.267</v>
       </c>
     </row>
     <row r="16">
@@ -970,37 +982,37 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>6.317</v>
+        <v>6.14</v>
       </c>
       <c r="C16" t="n">
-        <v>8.08</v>
+        <v>7.975</v>
       </c>
       <c r="D16" t="n">
-        <v>8.986000000000001</v>
+        <v>7.592</v>
       </c>
       <c r="E16" t="n">
-        <v>5.247</v>
+        <v>5.447</v>
       </c>
       <c r="F16" t="n">
-        <v>7.485</v>
+        <v>7.442</v>
       </c>
       <c r="G16" t="n">
-        <v>7.618</v>
+        <v>7.976</v>
       </c>
       <c r="H16" t="n">
-        <v>7.086</v>
+        <v>7.906</v>
       </c>
       <c r="I16" t="n">
-        <v>4.742</v>
+        <v>1.114</v>
       </c>
       <c r="J16" t="n">
-        <v>7.15</v>
+        <v>5.745</v>
       </c>
       <c r="K16" t="n">
-        <v>8.843</v>
+        <v>8.676</v>
       </c>
       <c r="L16" t="n">
-        <v>5.932</v>
+        <v>4.435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated new Media sector and trades from Fall 2020
</commit_message>
<xml_diff>
--- a/outputs/sectorbreakdown.xlsx
+++ b/outputs/sectorbreakdown.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -419,6 +419,11 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>Media</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Fixed Income</t>
         </is>
       </c>
@@ -430,37 +435,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.169</v>
+        <v>-1.357</v>
       </c>
       <c r="C2" t="n">
-        <v>3.406</v>
+        <v>-0.418</v>
       </c>
       <c r="D2" t="n">
-        <v>6.72</v>
+        <v>-13.513</v>
       </c>
       <c r="E2" t="n">
-        <v>-7.431</v>
+        <v>-2.211</v>
       </c>
       <c r="F2" t="n">
-        <v>5.361</v>
+        <v>-15.323</v>
       </c>
       <c r="G2" t="n">
-        <v>7.388</v>
+        <v>-0.671</v>
       </c>
       <c r="H2" t="n">
-        <v>-7.003</v>
+        <v>-1.063</v>
       </c>
       <c r="I2" t="n">
-        <v>-8.436999999999999</v>
+        <v>-2.419</v>
       </c>
       <c r="J2" t="n">
-        <v>11.294</v>
+        <v>-6.62</v>
       </c>
       <c r="K2" t="n">
-        <v>13.503</v>
+        <v>-3.21</v>
       </c>
       <c r="L2" t="n">
-        <v>1.849</v>
+        <v>-5.118</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.857</v>
       </c>
     </row>
     <row r="3">
@@ -470,37 +478,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-8.271000000000001</v>
+        <v>2.161</v>
       </c>
       <c r="C3" t="n">
-        <v>-12.956</v>
+        <v>14.271</v>
       </c>
       <c r="D3" t="n">
-        <v>-30.77</v>
+        <v>-16.967</v>
       </c>
       <c r="E3" t="n">
-        <v>-26.267</v>
+        <v>0.261</v>
       </c>
       <c r="F3" t="n">
-        <v>-19.926</v>
+        <v>-8.663</v>
       </c>
       <c r="G3" t="n">
-        <v>-12.543</v>
+        <v>12.287</v>
       </c>
       <c r="H3" t="n">
-        <v>-46.571</v>
+        <v>5.043</v>
       </c>
       <c r="I3" t="n">
-        <v>-34.373</v>
+        <v>18.754</v>
       </c>
       <c r="J3" t="n">
-        <v>-1.492</v>
+        <v>-0.296</v>
       </c>
       <c r="K3" t="n">
-        <v>-3.074</v>
+        <v>7.892</v>
       </c>
       <c r="L3" t="n">
-        <v>-18.034</v>
+        <v>-4.058</v>
+      </c>
+      <c r="M3" t="n">
+        <v>5.449</v>
       </c>
     </row>
     <row r="4">
@@ -510,37 +521,40 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-9.782</v>
+        <v>-12.295</v>
       </c>
       <c r="C4" t="n">
-        <v>-8.561</v>
+        <v>9.16</v>
       </c>
       <c r="D4" t="n">
-        <v>-28.539</v>
+        <v>-34.716</v>
       </c>
       <c r="E4" t="n">
-        <v>-18.944</v>
+        <v>-5.528</v>
       </c>
       <c r="F4" t="n">
-        <v>-15.487</v>
+        <v>-14.427</v>
       </c>
       <c r="G4" t="n">
-        <v>-7.514</v>
+        <v>4.975</v>
       </c>
       <c r="H4" t="n">
-        <v>-43.338</v>
+        <v>-32.25</v>
       </c>
       <c r="I4" t="n">
-        <v>-28.168</v>
+        <v>-7.425</v>
       </c>
       <c r="J4" t="n">
-        <v>-3.654</v>
+        <v>-9.298</v>
       </c>
       <c r="K4" t="n">
-        <v>6.349</v>
+        <v>24.154</v>
       </c>
       <c r="L4" t="n">
-        <v>-14.58</v>
+        <v>-6.717</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-2.206</v>
       </c>
     </row>
     <row r="5">
@@ -550,37 +564,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-8.156000000000001</v>
+        <v>-8.537000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>1.379</v>
+        <v>14.316</v>
       </c>
       <c r="D5" t="n">
-        <v>-30.691</v>
+        <v>-33.963</v>
       </c>
       <c r="E5" t="n">
-        <v>-8.654</v>
+        <v>1.783</v>
       </c>
       <c r="F5" t="n">
-        <v>-11.97</v>
+        <v>-14.32</v>
       </c>
       <c r="G5" t="n">
-        <v>1.614</v>
+        <v>11.84</v>
       </c>
       <c r="H5" t="n">
-        <v>-35.762</v>
+        <v>-28.917</v>
       </c>
       <c r="I5" t="n">
-        <v>-18.721</v>
+        <v>-4.489</v>
       </c>
       <c r="J5" t="n">
-        <v>6.867</v>
+        <v>-1.983</v>
       </c>
       <c r="K5" t="n">
-        <v>18.768</v>
+        <v>30.055</v>
       </c>
       <c r="L5" t="n">
-        <v>-16.698</v>
+        <v>-0.755</v>
+      </c>
+      <c r="M5" t="n">
+        <v>5.059</v>
       </c>
     </row>
     <row r="6">
@@ -590,37 +607,40 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-1.446</v>
+        <v>-8.446</v>
       </c>
       <c r="C6" t="n">
-        <v>46.582</v>
+        <v>40.174</v>
       </c>
       <c r="D6" t="n">
-        <v>-34.693</v>
+        <v>-40.337</v>
       </c>
       <c r="E6" t="n">
-        <v>35.836</v>
+        <v>58.315</v>
       </c>
       <c r="F6" t="n">
-        <v>37.168</v>
+        <v>-25.232</v>
       </c>
       <c r="G6" t="n">
-        <v>19.902</v>
+        <v>36.093</v>
       </c>
       <c r="H6" t="n">
-        <v>-40.495</v>
+        <v>-29.178</v>
       </c>
       <c r="I6" t="n">
-        <v>-7.879</v>
+        <v>18.723</v>
       </c>
       <c r="J6" t="n">
-        <v>18.361</v>
+        <v>5.33</v>
       </c>
       <c r="K6" t="n">
-        <v>94.608</v>
+        <v>119.843</v>
       </c>
       <c r="L6" t="n">
-        <v>-20.371</v>
+        <v>54.679</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-8.837</v>
       </c>
     </row>
     <row r="7">
@@ -630,37 +650,40 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.314</v>
+        <v>-1.767</v>
       </c>
       <c r="C7" t="n">
-        <v>8.621</v>
+        <v>7.06</v>
       </c>
       <c r="D7" t="n">
-        <v>-8.801</v>
+        <v>-9.906000000000001</v>
       </c>
       <c r="E7" t="n">
-        <v>6.847</v>
+        <v>9.724</v>
       </c>
       <c r="F7" t="n">
-        <v>7.073</v>
+        <v>-5.704</v>
       </c>
       <c r="G7" t="n">
-        <v>4.003</v>
+        <v>6.423</v>
       </c>
       <c r="H7" t="n">
-        <v>-10.618</v>
+        <v>-6.731</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.759</v>
+        <v>3.527</v>
       </c>
       <c r="J7" t="n">
-        <v>3.712</v>
+        <v>1.054</v>
       </c>
       <c r="K7" t="n">
-        <v>15.485</v>
+        <v>17.248</v>
       </c>
       <c r="L7" t="n">
-        <v>-4.806</v>
+        <v>9.210000000000001</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-1.851</v>
       </c>
     </row>
     <row r="8">
@@ -670,37 +693,40 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.756</v>
+        <v>0.85</v>
       </c>
       <c r="C8" t="n">
-        <v>0.985</v>
+        <v>0.978</v>
       </c>
       <c r="D8" t="n">
-        <v>1.044</v>
+        <v>1.075</v>
       </c>
       <c r="E8" t="n">
-        <v>0.979</v>
+        <v>0.971</v>
       </c>
       <c r="F8" t="n">
-        <v>1.009</v>
+        <v>1.03</v>
       </c>
       <c r="G8" t="n">
-        <v>1.035</v>
+        <v>1.02</v>
       </c>
       <c r="H8" t="n">
-        <v>1.115</v>
+        <v>1.119</v>
       </c>
       <c r="I8" t="n">
-        <v>0.859</v>
+        <v>0.881</v>
       </c>
       <c r="J8" t="n">
-        <v>0.612</v>
+        <v>0.893</v>
       </c>
       <c r="K8" t="n">
-        <v>1.039</v>
+        <v>1.063</v>
       </c>
       <c r="L8" t="n">
-        <v>0.604</v>
+        <v>0.952</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.598</v>
       </c>
     </row>
     <row r="9">
@@ -710,37 +736,40 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-6.515</v>
+        <v>-8.669</v>
       </c>
       <c r="C9" t="n">
-        <v>0.734</v>
+        <v>-0.781</v>
       </c>
       <c r="D9" t="n">
-        <v>-17.124</v>
+        <v>-18.459</v>
       </c>
       <c r="E9" t="n">
-        <v>-1.002</v>
+        <v>1.933</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.996</v>
+        <v>-13.926</v>
       </c>
       <c r="G9" t="n">
-        <v>-4.255</v>
+        <v>-1.722</v>
       </c>
       <c r="H9" t="n">
-        <v>-19.462</v>
+        <v>-15.601</v>
       </c>
       <c r="I9" t="n">
-        <v>-8.720000000000001</v>
+        <v>-3.601</v>
       </c>
       <c r="J9" t="n">
-        <v>-1.435</v>
+        <v>-6.16</v>
       </c>
       <c r="K9" t="n">
-        <v>7.196</v>
+        <v>8.788</v>
       </c>
       <c r="L9" t="n">
-        <v>-9.891</v>
+        <v>1.564</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-6.908</v>
       </c>
     </row>
     <row r="10">
@@ -750,37 +779,40 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.054</v>
+        <v>-0.128</v>
       </c>
       <c r="C10" t="n">
-        <v>0.394</v>
+        <v>0.267</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.291</v>
+        <v>-0.319</v>
       </c>
       <c r="E10" t="n">
-        <v>0.255</v>
+        <v>0.369</v>
       </c>
       <c r="F10" t="n">
-        <v>0.292</v>
+        <v>-0.201</v>
       </c>
       <c r="G10" t="n">
-        <v>0.138</v>
+        <v>0.237</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.412</v>
+        <v>-0.27</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.097</v>
+        <v>0.113</v>
       </c>
       <c r="J10" t="n">
-        <v>0.269</v>
+        <v>0.02</v>
       </c>
       <c r="K10" t="n">
-        <v>0.621</v>
+        <v>0.577</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.428</v>
+        <v>0.392</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-0.204</v>
       </c>
     </row>
     <row r="11">
@@ -790,37 +822,40 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.013</v>
+        <v>-0.029</v>
       </c>
       <c r="C11" t="n">
-        <v>0.081</v>
+        <v>0.065</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.09</v>
+        <v>-0.098</v>
       </c>
       <c r="E11" t="n">
-        <v>0.063</v>
+        <v>0.093</v>
       </c>
       <c r="F11" t="n">
-        <v>0.064</v>
+        <v>-0.062</v>
       </c>
       <c r="G11" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-0.066</v>
+      </c>
+      <c r="I11" t="n">
         <v>0.032</v>
       </c>
-      <c r="H11" t="n">
-        <v>-0.101</v>
-      </c>
-      <c r="I11" t="n">
-        <v>-0.028</v>
-      </c>
       <c r="J11" t="n">
-        <v>0.05</v>
+        <v>0.004</v>
       </c>
       <c r="K11" t="n">
-        <v>0.143</v>
+        <v>0.156</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.09</v>
+        <v>0.09</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-0.042</v>
       </c>
     </row>
     <row r="12">
@@ -830,10 +865,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-39.365</v>
+        <v>-46.362</v>
       </c>
       <c r="C12" t="n">
-        <v>-32.427</v>
+        <v>-44.163</v>
       </c>
       <c r="D12" t="n">
         <v>-66.36499999999999</v>
@@ -842,7 +877,7 @@
         <v>-44.101</v>
       </c>
       <c r="F12" t="n">
-        <v>-39.541</v>
+        <v>-53.669</v>
       </c>
       <c r="G12" t="n">
         <v>-36.075</v>
@@ -854,13 +889,16 @@
         <v>-42.377</v>
       </c>
       <c r="J12" t="n">
-        <v>-22.737</v>
+        <v>-43.677</v>
       </c>
       <c r="K12" t="n">
-        <v>-34.126</v>
+        <v>-39.753</v>
       </c>
       <c r="L12" t="n">
-        <v>-34.779</v>
+        <v>-35.67</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-34.782</v>
       </c>
     </row>
     <row r="13">
@@ -870,37 +908,40 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17.826</v>
+        <v>19.118</v>
       </c>
       <c r="C13" t="n">
-        <v>20.25</v>
+        <v>23.976</v>
       </c>
       <c r="D13" t="n">
-        <v>32.513</v>
+        <v>33.217</v>
       </c>
       <c r="E13" t="n">
-        <v>24.33</v>
+        <v>24.559</v>
       </c>
       <c r="F13" t="n">
-        <v>22.009</v>
+        <v>31.731</v>
       </c>
       <c r="G13" t="n">
-        <v>24.327</v>
+        <v>24.251</v>
       </c>
       <c r="H13" t="n">
-        <v>27.329</v>
+        <v>27.382</v>
       </c>
       <c r="I13" t="n">
-        <v>24.775</v>
+        <v>25.248</v>
       </c>
       <c r="J13" t="n">
-        <v>11.445</v>
+        <v>19.048</v>
       </c>
       <c r="K13" t="n">
-        <v>23.917</v>
+        <v>28.76</v>
       </c>
       <c r="L13" t="n">
-        <v>12.739</v>
+        <v>21.804</v>
+      </c>
+      <c r="M13" t="n">
+        <v>12.393</v>
       </c>
     </row>
     <row r="14">
@@ -910,37 +951,40 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.344</v>
+        <v>0.45</v>
       </c>
       <c r="C14" t="n">
-        <v>0.761</v>
+        <v>0.498</v>
       </c>
       <c r="D14" t="n">
         <v>0.471</v>
       </c>
       <c r="E14" t="n">
-        <v>0.416</v>
+        <v>0.422</v>
       </c>
       <c r="F14" t="n">
-        <v>0.791</v>
+        <v>0.393</v>
       </c>
       <c r="G14" t="n">
-        <v>0.519</v>
+        <v>0.512</v>
       </c>
       <c r="H14" t="n">
         <v>0.471</v>
       </c>
       <c r="I14" t="n">
-        <v>0.32</v>
+        <v>0.326</v>
       </c>
       <c r="J14" t="n">
-        <v>0.375</v>
+        <v>0.607</v>
       </c>
       <c r="K14" t="n">
-        <v>0.742</v>
+        <v>0.593</v>
       </c>
       <c r="L14" t="n">
-        <v>0.288</v>
+        <v>0.674</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.296</v>
       </c>
     </row>
     <row r="15">
@@ -950,37 +994,40 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>6.201</v>
+        <v>6.902</v>
       </c>
       <c r="C15" t="n">
-        <v>7.887</v>
+        <v>7.84</v>
       </c>
       <c r="D15" t="n">
-        <v>8.321999999999999</v>
+        <v>8.552</v>
       </c>
       <c r="E15" t="n">
-        <v>7.849</v>
+        <v>7.791</v>
       </c>
       <c r="F15" t="n">
-        <v>8.069000000000001</v>
+        <v>8.221</v>
       </c>
       <c r="G15" t="n">
-        <v>8.257999999999999</v>
+        <v>8.145</v>
       </c>
       <c r="H15" t="n">
-        <v>8.843999999999999</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="I15" t="n">
-        <v>6.961</v>
+        <v>7.128</v>
       </c>
       <c r="J15" t="n">
-        <v>5.147</v>
+        <v>7.214</v>
       </c>
       <c r="K15" t="n">
-        <v>8.289</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="L15" t="n">
-        <v>5.085</v>
+        <v>7.646</v>
+      </c>
+      <c r="M15" t="n">
+        <v>5.057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing code/files to be most up-to-date
</commit_message>
<xml_diff>
--- a/outputs/sectorbreakdown.xlsx
+++ b/outputs/sectorbreakdown.xlsx
@@ -498,37 +498,37 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>9.292999999999999</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>10.62</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>20.554</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1.535</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>16.886</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1.842</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>17.998</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0.712</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>10.958</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>13.419</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>5.994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -536,37 +536,37 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>-2.584</v>
+        <v>9.933999999999999</v>
       </c>
       <c r="C3">
-        <v>4.693</v>
+        <v>9.170999999999999</v>
       </c>
       <c r="D3">
-        <v>17.316</v>
+        <v>29.139</v>
       </c>
       <c r="E3">
-        <v>-0.263</v>
+        <v>6.129</v>
       </c>
       <c r="F3">
-        <v>13.204</v>
+        <v>20.462</v>
       </c>
       <c r="G3">
-        <v>7.782</v>
+        <v>3.047</v>
       </c>
       <c r="H3">
-        <v>12.04</v>
+        <v>22.093</v>
       </c>
       <c r="I3">
-        <v>13.731</v>
+        <v>2.294</v>
       </c>
       <c r="K3">
-        <v>1.648</v>
+        <v>8.565</v>
       </c>
       <c r="L3">
-        <v>12.883</v>
+        <v>17.975</v>
       </c>
       <c r="M3">
-        <v>3.897</v>
+        <v>6.507</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -574,37 +574,37 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>-11.281</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>24.152</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>-33.442</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>2.688</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>17.536</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>12.437</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>-5.218</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>9.122</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>45.99</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>27.766</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>4.087</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -612,37 +612,37 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>-11.52</v>
+        <v>-11.019</v>
       </c>
       <c r="C5">
-        <v>29.75</v>
+        <v>23.664</v>
       </c>
       <c r="D5">
-        <v>-31.262</v>
+        <v>-28.644</v>
       </c>
       <c r="E5">
-        <v>8.071</v>
+        <v>-1.191</v>
       </c>
       <c r="F5">
-        <v>18.427</v>
+        <v>15.26</v>
       </c>
       <c r="G5">
-        <v>14.611</v>
+        <v>10.569</v>
       </c>
       <c r="H5">
-        <v>-1.958</v>
+        <v>-7.81</v>
       </c>
       <c r="I5">
-        <v>12.281</v>
+        <v>5.096</v>
       </c>
       <c r="K5">
-        <v>54.151</v>
+        <v>40.579</v>
       </c>
       <c r="L5">
-        <v>32.404</v>
+        <v>26.442</v>
       </c>
       <c r="M5">
-        <v>5.805</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -726,37 +726,37 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>0.783</v>
+        <v>0.779</v>
       </c>
       <c r="C8">
-        <v>1.01</v>
+        <v>1.002</v>
       </c>
       <c r="D8">
-        <v>1.136</v>
+        <v>1.128</v>
       </c>
       <c r="E8">
-        <v>0.9340000000000001</v>
+        <v>0.928</v>
       </c>
       <c r="F8">
-        <v>1.076</v>
+        <v>1.068</v>
       </c>
       <c r="G8">
-        <v>1.003</v>
+        <v>0.996</v>
       </c>
       <c r="H8">
-        <v>1.044</v>
+        <v>1.036</v>
       </c>
       <c r="I8">
-        <v>0.797</v>
+        <v>0.792</v>
       </c>
       <c r="K8">
-        <v>1.009</v>
+        <v>1.002</v>
       </c>
       <c r="L8">
-        <v>0.956</v>
+        <v>0.95</v>
       </c>
       <c r="M8">
-        <v>0.5600000000000001</v>
+        <v>0.5580000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -764,37 +764,37 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>-6.436</v>
+        <v>-6.433</v>
       </c>
       <c r="C9">
-        <v>12.152</v>
+        <v>12.204</v>
       </c>
       <c r="D9">
-        <v>-17.05</v>
+        <v>-16.972</v>
       </c>
       <c r="E9">
-        <v>11.997</v>
+        <v>12.032</v>
       </c>
       <c r="F9">
-        <v>9.992000000000001</v>
+        <v>10.055</v>
       </c>
       <c r="G9">
-        <v>0.315</v>
+        <v>0.364</v>
       </c>
       <c r="H9">
-        <v>-6.734</v>
+        <v>-6.676</v>
       </c>
       <c r="I9">
-        <v>4.691</v>
+        <v>4.701</v>
       </c>
       <c r="K9">
-        <v>19.042</v>
+        <v>19.095</v>
       </c>
       <c r="L9">
-        <v>8.849</v>
+        <v>8.887</v>
       </c>
       <c r="M9">
-        <v>-2.766</v>
+        <v>-2.806</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -802,37 +802,37 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <v>-0.046</v>
+        <v>-0.053</v>
       </c>
       <c r="C10">
-        <v>0.911</v>
+        <v>0.905</v>
       </c>
       <c r="D10">
-        <v>-0.294</v>
+        <v>-0.298</v>
       </c>
       <c r="E10">
-        <v>0.766</v>
+        <v>0.761</v>
       </c>
       <c r="F10">
-        <v>0.767</v>
+        <v>0.761</v>
       </c>
       <c r="G10">
-        <v>0.308</v>
+        <v>0.303</v>
       </c>
       <c r="H10">
-        <v>0.028</v>
+        <v>0.022</v>
       </c>
       <c r="I10">
-        <v>0.455</v>
+        <v>0.449</v>
       </c>
       <c r="K10">
-        <v>0.947</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="L10">
-        <v>0.74</v>
+        <v>0.734</v>
       </c>
       <c r="M10">
-        <v>0.121</v>
+        <v>0.108</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -840,13 +840,13 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>-0.011</v>
+        <v>-0.013</v>
       </c>
       <c r="C11">
         <v>0.191</v>
       </c>
       <c r="D11">
-        <v>-0.079</v>
+        <v>-0.081</v>
       </c>
       <c r="E11">
         <v>0.199</v>
@@ -855,22 +855,22 @@
         <v>0.164</v>
       </c>
       <c r="G11">
-        <v>0.074</v>
+        <v>0.073</v>
       </c>
       <c r="H11">
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="I11">
-        <v>0.13</v>
+        <v>0.129</v>
       </c>
       <c r="K11">
-        <v>0.259</v>
+        <v>0.26</v>
       </c>
       <c r="L11">
         <v>0.163</v>
       </c>
       <c r="M11">
-        <v>0.021</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -957,37 +957,37 @@
         <v>24</v>
       </c>
       <c r="B14">
-        <v>0.391</v>
+        <v>0.398</v>
       </c>
       <c r="C14">
-        <v>0.713</v>
+        <v>0.727</v>
       </c>
       <c r="D14">
-        <v>0.457</v>
+        <v>0.466</v>
       </c>
       <c r="E14">
-        <v>0.458</v>
+        <v>0.467</v>
       </c>
       <c r="F14">
-        <v>0.819</v>
+        <v>0.836</v>
       </c>
       <c r="G14">
-        <v>0.509</v>
+        <v>0.519</v>
       </c>
       <c r="H14">
-        <v>0.5629999999999999</v>
+        <v>0.575</v>
       </c>
       <c r="I14">
-        <v>0.373</v>
+        <v>0.381</v>
       </c>
       <c r="K14">
-        <v>0.62</v>
+        <v>0.633</v>
       </c>
       <c r="L14">
-        <v>0.731</v>
+        <v>0.745</v>
       </c>
       <c r="M14">
-        <v>0.322</v>
+        <v>0.329</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -995,37 +995,37 @@
         <v>25</v>
       </c>
       <c r="B15">
-        <v>6.467</v>
+        <v>6.464</v>
       </c>
       <c r="C15">
-        <v>8.068</v>
+        <v>8.016</v>
       </c>
       <c r="D15">
-        <v>8.965999999999999</v>
+        <v>8.888</v>
       </c>
       <c r="E15">
-        <v>7.535</v>
+        <v>7.5</v>
       </c>
       <c r="F15">
-        <v>8.535</v>
+        <v>8.472</v>
       </c>
       <c r="G15">
-        <v>8.02</v>
+        <v>7.971</v>
       </c>
       <c r="H15">
-        <v>8.311999999999999</v>
+        <v>8.254</v>
       </c>
       <c r="I15">
-        <v>6.565</v>
+        <v>6.555</v>
       </c>
       <c r="K15">
-        <v>8.066000000000001</v>
+        <v>8.012</v>
       </c>
       <c r="L15">
-        <v>7.69</v>
+        <v>7.652</v>
       </c>
       <c r="M15">
-        <v>4.886</v>
+        <v>4.926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>